<commit_message>
Ruth de León - Modified LOGT Form (C2)
</commit_message>
<xml_diff>
--- a/Organización Proyecto/Corte 2/Programacion/Ruth de León - Formulario LOGT (C2).xlsx
+++ b/Organización Proyecto/Corte 2/Programacion/Ruth de León - Formulario LOGT (C2).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Formulario LOGT (C2)</t>
   </si>
@@ -112,9 +112,6 @@
     <t>2:44 PM</t>
   </si>
   <si>
-    <t>0 min</t>
-  </si>
-  <si>
     <t>8 mins</t>
   </si>
   <si>
@@ -149,15 +146,35 @@
   </si>
   <si>
     <t>Se le da algunos detalles al informe para que este organizado</t>
+  </si>
+  <si>
+    <t>9:47 AM</t>
+  </si>
+  <si>
+    <t>9:53 AM</t>
+  </si>
+  <si>
+    <t>Se agregan los formularios LOGT</t>
+  </si>
+  <si>
+    <t>9:54 AM</t>
+  </si>
+  <si>
+    <t>10:28 AM</t>
+  </si>
+  <si>
+    <t>34 mins</t>
+  </si>
+  <si>
+    <t>Se modifican un par de casos de usos a los roles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;/&quot;mm&quot;/&quot;yy"/>
-    <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -267,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -295,9 +312,6 @@
     </xf>
     <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,16 +693,16 @@
         <v>32</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12">
@@ -696,22 +710,22 @@
         <v>45344.0</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="11" t="s">
+      <c r="H12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13">
@@ -719,41 +733,69 @@
         <v>45345.0</v>
       </c>
       <c r="D13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>14</v>
       </c>
       <c r="I13" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" s="10">
+        <v>45346.0</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="E14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15">
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="C15" s="10">
+        <v>45346.0</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>